<commit_message>
Ajustando caminhos para bloco 2 no térreo
</commit_message>
<xml_diff>
--- a/src/main/resources/Planilha_Locais.xlsx
+++ b/src/main/resources/Planilha_Locais.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osmar\git\IFSCMapRoutingWS\MapeamentoIFSC\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osmar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447B1464-F891-4963-96A6-0507F942E624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441BF22F-36E4-4BBB-9EA5-C88F391CE4F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AZ93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AZ93" sqref="AZ93"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AW40" sqref="AW40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1036,7 +1036,7 @@
         <v>37</v>
       </c>
       <c r="G40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H40">
         <v>2</v>
@@ -1048,22 +1048,22 @@
         <v>2</v>
       </c>
       <c r="S40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z40">
         <v>2</v>

</xml_diff>